<commit_message>
Added a new use case text desc.
Now view menu is a use case and sub-use case of make order.
</commit_message>
<xml_diff>
--- a/Planning/Use Case Text Description.xlsx
+++ b/Planning/Use Case Text Description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simpl\Dropbox\Advanced Software Engineering\CW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simpl\Dropbox\Advanced Software Engineering\CW\Advanced_Software_Engineering\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0312C315-9F65-461F-91A4-82549A2BEBF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD07FB78-772A-4173-BE7B-8BC166FBC06C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{F1D5681B-4D44-442C-9850-D4DEB156732B}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Actors</t>
   </si>
   <si>
-    <t>Sales staff</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -78,48 +75,21 @@
     <t>Café is open</t>
   </si>
   <si>
-    <t>1. List of available items is displayed</t>
-  </si>
-  <si>
     <t>2. One or more item is selected to order</t>
   </si>
   <si>
-    <t>3. Available discounts are shown</t>
-  </si>
-  <si>
-    <t>4. Order is submitted</t>
-  </si>
-  <si>
-    <t>5. Discount is applied</t>
-  </si>
-  <si>
-    <t>6. Order is added to list of orders</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1. Order is not submitted</t>
   </si>
   <si>
     <t xml:space="preserve">  2. Prompt user to enter at least one item then continue from 2</t>
   </si>
   <si>
-    <t>4a. No items are selected</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1. Discount is displayed as zero</t>
   </si>
   <si>
-    <t>3a. Order does not qualify for any discounts</t>
-  </si>
-  <si>
-    <t>5a. Order does not qualify for any discounts</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1. Continue from 6</t>
   </si>
   <si>
-    <t>6. Order can not be added to list of orders</t>
-  </si>
-  <si>
     <t xml:space="preserve">  1. User is informed order has not been added</t>
   </si>
   <si>
@@ -169,6 +139,69 @@
   </si>
   <si>
     <t>Report has been created</t>
+  </si>
+  <si>
+    <t>View available items and prices</t>
+  </si>
+  <si>
+    <t>1. View list of available items</t>
+  </si>
+  <si>
+    <t>View Menu</t>
+  </si>
+  <si>
+    <t>Includes view menu</t>
+  </si>
+  <si>
+    <t>2. Select one or more item</t>
+  </si>
+  <si>
+    <t>3. Total price is shown</t>
+  </si>
+  <si>
+    <t>4. Available discounts are shown</t>
+  </si>
+  <si>
+    <t>5. Order is submitted</t>
+  </si>
+  <si>
+    <t>6. Discount is applied</t>
+  </si>
+  <si>
+    <t>7. Order is added to list of orders</t>
+  </si>
+  <si>
+    <t>6a. Order does not qualify for any discounts</t>
+  </si>
+  <si>
+    <t>7a. Order can not be added to list of orders</t>
+  </si>
+  <si>
+    <t>5a. No items are selected</t>
+  </si>
+  <si>
+    <t>4a. Order does not qualify for any discounts</t>
+  </si>
+  <si>
+    <t>3.Total price is shown</t>
+  </si>
+  <si>
+    <t>1a. No item data to display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1. Menu is blank</t>
+  </si>
+  <si>
+    <t>1. List items browsed (sub use case)</t>
+  </si>
+  <si>
+    <t>Sales Assistant, Customer</t>
+  </si>
+  <si>
+    <t>Sales assistant, Customer</t>
+  </si>
+  <si>
+    <t>Customer</t>
   </si>
 </sst>
 </file>
@@ -200,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -223,11 +256,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -244,16 +303,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,314 +653,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD19EB9-9988-4F0A-AF12-A3BC596891EB}">
-  <dimension ref="B2:H27"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="41.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="F7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="F10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="I10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="F11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="I11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="F12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="F13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="F14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="I14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="F15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="I15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="F16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="G16" s="10"/>
+      <c r="I16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="F17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="E6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="E7" s="7" t="s">
+      <c r="G17" s="4"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="F18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="G18" s="10"/>
+      <c r="I18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="F19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="F20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="E9" s="5" t="s">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="F21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="E11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="E13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="E14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="E15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="E16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="E17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="E18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="E19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="E20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="D26" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
+  <mergeCells count="45">
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>